<commit_message>
White wines in menu
</commit_message>
<xml_diff>
--- a/menu_files/166825177696027.xlsx
+++ b/menu_files/166825177696027.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1314,6 +1314,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ФРЕШ-ВІТАМІННІ МІКСИ
 </t>
@@ -1325,6 +1326,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Яблучно-морквяний
 Апельсиново-морквяно-буряковий Селерово-буряково-яблучний Грейпфрутово-медово-грушевий Імбирно-селерово-апельсиновий Апельсиновий
@@ -1441,6 +1443,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">КОКТЕЙЛІ
 </t>
@@ -1451,6 +1454,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">АЛКОГОЛЬНІ</t>
     </r>
@@ -1466,6 +1470,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ванільний сироп, текіла, ром, джин, кола, лимонний сік)
 </t>
@@ -1477,6 +1482,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Berry Killer</t>
     </r>
@@ -1492,6 +1498,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">малиновий сироп, лимонний сік, полуниця, смородина, м’ята)
 </t>
@@ -1503,6 +1510,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Blue Lagoon</t>
     </r>
@@ -1515,6 +1523,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(горілка, лікер Blue Curacao, Sprite, лимон)
 </t>
@@ -1526,6 +1535,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Cosmopolitan</t>
     </r>
@@ -1538,6 +1548,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(горілка, лікер, сік)
 </t>
@@ -1549,6 +1560,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Sex on Beach</t>
     </r>
@@ -1561,6 +1573,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(горілка, лікер, гранатовий сироп, сік)
 </t>
@@ -1572,6 +1585,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Hungarian Merry</t>
     </r>
@@ -1584,6 +1598,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(горілка, томатний сік, Ерош Пішта, сіль, чорний перець, лід)
 </t>
@@ -1595,6 +1610,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Pina Colada</t>
     </r>
@@ -1607,6 +1623,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(ром, лікер Malibu, кокосовий сироп, вершки, ананасовий сік)
 </t>
@@ -1618,6 +1635,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mojito</t>
     </r>
@@ -1630,6 +1648,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">( ром, Sprite, лайм, м’ята, тростниковий цукор)
 </t>
@@ -1641,6 +1660,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Jin-Tonic</t>
     </r>
@@ -1653,6 +1673,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(джин, тонік, лайм)
 </t>
@@ -1664,6 +1685,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Margarita</t>
     </r>
@@ -1676,6 +1698,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(текіла, лікер, сіль, лайм, лимонний сік)
 </t>
@@ -1687,6 +1710,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Tequila Sunrise</t>
     </r>
@@ -1699,6 +1723,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(текіла, ананасовий сік, гранатовий сироп, апельсин)
 </t>
@@ -1710,6 +1735,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Strawberry Punch</t>
     </r>
@@ -1722,6 +1748,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Prosecco, ром, сік, полуниця, лайм, лід)
 </t>
@@ -1733,6 +1760,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Aperol</t>
     </r>
@@ -1745,6 +1773,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Prosecco , лікер Aperol, апельсин)
 </t>
@@ -1756,6 +1785,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Martini Royal</t>
     </r>
@@ -1768,6 +1798,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(білий вермут, Prosecco, лаймовий сік, лайм, м’ята, лід)
 </t>
@@ -1779,6 +1810,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Penicillin</t>
     </r>
@@ -1791,6 +1823,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(віскі, сироп, мед, лимонний фреш, імбир)
 </t>
@@ -1802,6 +1835,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Hugo Sprits</t>
     </r>
@@ -1814,6 +1848,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(вино, Prosecco, сироп, лайм, м’ята)
 </t>
@@ -1825,6 +1860,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Negroni</t>
     </r>
@@ -1837,6 +1873,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(джин, апероль, вермут)
 </t>
@@ -1848,6 +1885,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Berry whiskey</t>
     </r>
@@ -1866,6 +1904,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(самбука, лікер Baileys, абсент)
 </t>
@@ -1877,6 +1916,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Лексус</t>
     </r>
@@ -1889,6 +1929,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(лікер Kahlua, самбука, лікер Baileys, лікер Blue Curacao)
 </t>
@@ -1900,6 +1941,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Б-52</t>
     </r>
@@ -1959,6 +2001,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">БІЛІ ВИНА
 </t>
@@ -1969,6 +2012,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">УКРАЇНА                                                </t>
     </r>
@@ -1978,6 +2022,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -1996,6 +2041,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Chateau Chizay Pinot Blanc                                            96,00 / 480,00
 </t>
@@ -2007,6 +2053,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Напівсолодке. Смак живий, легкий, елегантний, добре збалансований, освіжаючий післясмак з легкою мінеральністю. Вино розкривається пишним букетом білих квітів, цитрусових, яблук з прянощами, медом і відтінками стиглих фруктів.)</t>
     </r>
@@ -2018,6 +2065,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ІТАЛІЯ                                                   </t>
     </r>
@@ -2027,6 +2075,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2045,6 +2094,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ІСПАНІЯ                                                </t>
     </r>
@@ -2054,6 +2104,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2072,6 +2123,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ФРАНЦІЯ                                               </t>
     </r>
@@ -2081,6 +2133,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2096,6 +2149,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Напівсолодке, виготовлене з сорту винограду Уні Блан, Совіньйон Блан. Аромат вина,
 сповнений  ніжними  фруктовими  та  медовими  нотками,  а  медовий  смак  сповнений чарівності фруктів з домінуючими нотами абрикоса.)
@@ -2107,6 +2161,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ЧІЛІ                                                     </t>
     </r>
@@ -2116,6 +2171,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2134,6 +2190,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Montes Chardonnay Reserva                                        180,00 / 900,00
 </t>
@@ -2145,6 +2202,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Сухе. Смак ідеально збалансований, маслянистий, складний, з довгим вершковим післясмаком. Аромат: квітково-фруктовий, з яскраво вираженим букетом тропічних фруктів, з елегантними вкрапленнями дуба, з ванільним і вершковим відтінком.)</t>
     </r>
@@ -2156,6 +2214,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">НОВА ЗЕЛАНДІЯ
 </t>
@@ -2167,6 +2226,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Marlborough Sun Sauvignon Blanc                              231,00 / 1155,00
 </t>
@@ -2178,6 +2238,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Сухе. Пишний аромат маракуї, аґрусу, листя чорної смородини в обрамленні тонких цитрусових тонів. У смаку добре збалансоване вино, має приємну свіжість з яскравим характером. Післясмак затяжний, освіжаючий.)</t>
     </r>
@@ -2189,6 +2250,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ЧЕРВОНІ ВИНА
 </t>
@@ -2199,6 +2261,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">УКРАЇНА                                                </t>
     </r>
@@ -2208,6 +2271,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2227,6 +2291,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Chateau Chizay Піно Нуар                                            96,00 / 480,00
 </t>
@@ -2238,6 +2303,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Напівсолодке.  Колір  вина  красивий  гранатовий,  аромат  –  яскравий  з  відтінками темних і червоних ягід. Приємний, злегка терпкий, ягідний смак з нотками вишні та малини завершується тривалим та гармонійним післясмаком.)
 </t>
@@ -2248,6 +2314,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ІТАЛІЯ                                                   </t>
     </r>
@@ -2257,6 +2324,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2282,6 +2350,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Entrecote, Gourmet Pere &amp; Fils                                      168,00 / 840,00
 </t>
@@ -2293,6 +2362,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Напівсухе. Смак м'який, гладкий, питкий, повнотілий, дуже соковитий, з оксамитови- ми танінами та гармонійною кислотністю, післясмак тривалий, приємний, з ягідними тонами. Аромат щедрий, багатий букет демонструє яскраві фруктові ноти слив, вишні, стиглої ожини з тонкими нюансами спецій.)</t>
     </r>
@@ -2305,6 +2375,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Reserve de l’Audbe Pere Anselme Syrah-Merlot, Brotte   120,00 / 600,00
 </t>
@@ -2316,6 +2387,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Сухе. Смак округлий, повнотілий, з приємною легкістю, гострими ягідними нотами і тривалим післясмаком. Аромат яскравий, соковитий, з нотами вишні, малини і легким нюансом ванілі.)</t>
     </r>
@@ -2327,6 +2399,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ЧІЛІ                                                      </t>
     </r>
@@ -2336,6 +2409,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2354,6 +2428,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ІСПАНІЯ                                                 </t>
     </r>
@@ -2363,6 +2438,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2381,6 +2457,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">АВСТРАЛІЯ                                             </t>
     </r>
@@ -2390,6 +2467,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2453,6 +2531,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">РОЖЕВІ ВИНА
 </t>
@@ -2463,6 +2542,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">НОВА ЗЕЛАНДІЯ                                       </t>
     </r>
@@ -2472,6 +2552,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2490,6 +2571,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ЧІЛІ                                                     </t>
     </r>
@@ -2499,6 +2581,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">150 мл / пл</t>
     </r>
@@ -2541,6 +2624,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ЧЕРВОНІ
 </t>
@@ -2552,6 +2636,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">La Foret Bourgogne Rouge AOC 2016 (Франція, 2016)</t>
     </r>
@@ -2563,6 +2648,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Microsoft Sans Serif"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">пляшка
 </t>
@@ -2574,6 +2660,7 @@
         <color rgb="FF3B2314"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1860,00</t>
     </r>
@@ -2649,6 +2736,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2670,6 +2758,7 @@
       <color rgb="FF3B2314"/>
       <name val="Microsoft Sans Serif"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2677,18 +2766,21 @@
       <color rgb="FF3B2314"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3B2314"/>
       <name val="Microsoft Sans Serif"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2696,6 +2788,7 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2703,12 +2796,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2716,12 +2811,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="26"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2729,12 +2826,14 @@
       <color rgb="FF3B2314"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="20"/>
       <color rgb="FF3B2314"/>
       <name val="Microsoft Sans Serif"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2742,6 +2841,7 @@
       <color rgb="FF3B2314"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2749,12 +2849,14 @@
       <color rgb="FF3B2314"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="20.5"/>
       <color rgb="FF3B2314"/>
       <name val="Microsoft Sans Serif"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2762,6 +2864,7 @@
       <color rgb="FF3B2314"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2769,6 +2872,7 @@
       <color rgb="FF3B2314"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2776,6 +2880,7 @@
       <color rgb="FF3B2314"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2844,7 +2949,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="82">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2854,7 +2959,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2870,7 +2975,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="12" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2886,7 +2991,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -3018,7 +3123,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="12" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3059,10 +3164,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="12" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3109,10 +3210,6 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="12" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3122,7 +3219,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3163,10 +3260,6 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="12" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3268,9 +3361,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1368360</xdr:colOff>
+      <xdr:colOff>1368000</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>4994280</xdr:rowOff>
+      <xdr:rowOff>4993920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3284,7 +3377,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3412080" y="8864280"/>
-          <a:ext cx="6586560" cy="10233000"/>
+          <a:ext cx="6586200" cy="10232640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3310,9 +3403,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>946440</xdr:colOff>
+      <xdr:colOff>946080</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>4993560</xdr:rowOff>
+      <xdr:rowOff>4993200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3326,7 +3419,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4230000" y="15836040"/>
-          <a:ext cx="6586200" cy="10233000"/>
+          <a:ext cx="6585840" cy="10232640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3352,9 +3445,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1354680</xdr:colOff>
+      <xdr:colOff>1354320</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>5018400</xdr:rowOff>
+      <xdr:rowOff>5018040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3368,7 +3461,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5117040" y="8332920"/>
-          <a:ext cx="6586560" cy="10233000"/>
+          <a:ext cx="6586200" cy="10232640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3394,9 +3487,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>756720</xdr:colOff>
+      <xdr:colOff>756360</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>5002560</xdr:rowOff>
+      <xdr:rowOff>5002200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3410,7 +3503,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3983760" y="5764320"/>
-          <a:ext cx="6586200" cy="10233000"/>
+          <a:ext cx="6585840" cy="10232640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3430,135 +3523,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>864720</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1354680</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>5039280</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="image1.png" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5370480" y="7569720"/>
-          <a:ext cx="6586560" cy="10233000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>252720</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>742680</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>5038920</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="image3.png" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4758480" y="25139520"/>
-          <a:ext cx="6586560" cy="10233000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>864720</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1354680</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>5039280</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="image1.png" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5370480" y="40980240"/>
-          <a:ext cx="6586560" cy="10233000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>252720</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>140400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1249200</xdr:colOff>
+      <xdr:colOff>1248840</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>4998240</xdr:rowOff>
+      <xdr:rowOff>4997880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="image4.png" descr=""/>
+        <xdr:cNvPr id="4" name="image4.png" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3568,7 +3545,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2955600" y="6372720"/>
-          <a:ext cx="6585840" cy="10233000"/>
+          <a:ext cx="6585480" cy="10232640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3589,13 +3566,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1861200</xdr:colOff>
+      <xdr:colOff>1860840</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>5039280</xdr:rowOff>
+      <xdr:rowOff>5038920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="image1.png" descr=""/>
+        <xdr:cNvPr id="5" name="image1.png" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3605,7 +3582,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3567600" y="20072880"/>
-          <a:ext cx="6585840" cy="10233000"/>
+          <a:ext cx="6585480" cy="10232640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3626,13 +3603,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1071000</xdr:colOff>
+      <xdr:colOff>1070640</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="image5.png" descr=""/>
+        <xdr:cNvPr id="6" name="image5.png" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3642,7 +3619,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2777400" y="21929400"/>
-          <a:ext cx="6585840" cy="10233000"/>
+          <a:ext cx="6585480" cy="10232640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3663,19 +3640,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1623240</xdr:colOff>
+      <xdr:colOff>1622880</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>52920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Shape 17"/>
+        <xdr:cNvPr id="7" name="Shape 17"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5112000" y="30818160"/>
-          <a:ext cx="1917360" cy="360"/>
+          <a:ext cx="1917000" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3719,13 +3696,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>173880</xdr:colOff>
+      <xdr:colOff>173520</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="image6.png" descr=""/>
+        <xdr:cNvPr id="8" name="image6.png" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3735,7 +3712,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5448960" y="30303720"/>
-          <a:ext cx="131040" cy="131040"/>
+          <a:ext cx="130680" cy="130680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3756,19 +3733,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2575080</xdr:colOff>
+      <xdr:colOff>2574720</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>360360</xdr:rowOff>
+      <xdr:rowOff>360000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Shape 19"/>
+        <xdr:cNvPr id="9" name="Shape 19"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5135400" y="30526200"/>
-          <a:ext cx="142560" cy="142560"/>
+          <a:ext cx="142200" cy="142200"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3988,10 +3965,10 @@
   <dimension ref="B1:F37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="1" sqref="A10:G13 B27"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="40.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.67"/>
@@ -4497,11 +4474,11 @@
   </sheetPr>
   <dimension ref="B1:E56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A10:G13 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="71.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.88"/>
@@ -4521,10 +4498,10 @@
       <c r="B2" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D2" s="73" t="n">
+      <c r="D2" s="71" t="n">
         <v>975</v>
       </c>
       <c r="E2" s="3"/>
@@ -4533,10 +4510,10 @@
       <c r="B3" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D3" s="73" t="n">
+      <c r="D3" s="71" t="n">
         <v>780</v>
       </c>
       <c r="E3" s="3"/>
@@ -4545,10 +4522,10 @@
       <c r="B4" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D4" s="73" t="n">
+      <c r="D4" s="71" t="n">
         <v>780</v>
       </c>
       <c r="E4" s="3"/>
@@ -4557,10 +4534,10 @@
       <c r="B5" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D5" s="73" t="n">
+      <c r="D5" s="71" t="n">
         <v>720</v>
       </c>
       <c r="E5" s="3"/>
@@ -4569,10 +4546,10 @@
       <c r="B6" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="C6" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D6" s="73" t="n">
+      <c r="D6" s="71" t="n">
         <v>700</v>
       </c>
       <c r="E6" s="3"/>
@@ -4581,10 +4558,10 @@
       <c r="B7" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D7" s="73" t="n">
+      <c r="D7" s="71" t="n">
         <v>700</v>
       </c>
       <c r="E7" s="3"/>
@@ -4593,10 +4570,10 @@
       <c r="B8" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D8" s="73" t="n">
+      <c r="D8" s="71" t="n">
         <v>380</v>
       </c>
       <c r="E8" s="3"/>
@@ -4605,10 +4582,10 @@
       <c r="B9" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D9" s="73" t="n">
+      <c r="D9" s="71" t="n">
         <v>380</v>
       </c>
       <c r="E9" s="3"/>
@@ -4617,10 +4594,10 @@
       <c r="B10" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D10" s="73" t="n">
+      <c r="D10" s="71" t="n">
         <v>300</v>
       </c>
       <c r="E10" s="3"/>
@@ -4629,10 +4606,10 @@
       <c r="B11" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D11" s="73" t="n">
+      <c r="D11" s="71" t="n">
         <v>390</v>
       </c>
       <c r="E11" s="3"/>
@@ -4641,10 +4618,10 @@
       <c r="B12" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="64" t="s">
         <v>338</v>
       </c>
-      <c r="D12" s="73" t="n">
+      <c r="D12" s="71" t="n">
         <v>390</v>
       </c>
       <c r="E12" s="3"/>
@@ -4653,10 +4630,10 @@
       <c r="B13" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="64" t="s">
         <v>393</v>
       </c>
-      <c r="D13" s="73" t="n">
+      <c r="D13" s="71" t="n">
         <v>110</v>
       </c>
       <c r="E13" s="3"/>
@@ -4678,28 +4655,28 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="72" t="s">
         <v>498</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
     </row>
     <row r="17" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="73" t="s">
         <v>499</v>
       </c>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
     </row>
     <row r="18" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="74" t="s">
         <v>500</v>
       </c>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="4" t="s">
@@ -4710,20 +4687,20 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="72" t="s">
         <v>502</v>
       </c>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
     </row>
     <row r="21" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="76" t="s">
+      <c r="B21" s="74" t="s">
         <v>503</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
     </row>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="4" t="s">
@@ -4734,82 +4711,82 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="72" t="s">
         <v>505</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-    </row>
-    <row r="24" customFormat="false" ht="409" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="397" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="77" t="s">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="75" t="s">
         <v>506</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-    </row>
-    <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="70" t="s">
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="68" t="s">
         <v>507</v>
       </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-    </row>
-    <row r="28" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="78" t="s">
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="76" t="s">
         <v>508</v>
       </c>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-    </row>
-    <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="70" t="s">
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="68" t="s">
         <v>509</v>
       </c>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-    </row>
-    <row r="30" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="74" t="s">
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="72" t="s">
         <v>510</v>
       </c>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-    </row>
-    <row r="31" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="75" t="s">
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="73" t="s">
         <v>511</v>
       </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-    </row>
-    <row r="32" customFormat="false" ht="94.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="76" t="s">
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="74" t="s">
         <v>512</v>
       </c>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-    </row>
-    <row r="33" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="9" t="s">
         <v>513</v>
       </c>
@@ -4817,67 +4794,67 @@
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="70" t="s">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="68" t="s">
         <v>514</v>
       </c>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-    </row>
-    <row r="35" customFormat="false" ht="43" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="74" t="s">
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="72" t="s">
         <v>515</v>
       </c>
-      <c r="C35" s="74"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="74"/>
-    </row>
-    <row r="36" customFormat="false" ht="89.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="75" t="s">
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="73" t="s">
         <v>516</v>
       </c>
-      <c r="C36" s="75"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-    </row>
-    <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="70" t="s">
+      <c r="C36" s="73"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="73"/>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="68" t="s">
         <v>517</v>
       </c>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-    </row>
-    <row r="38" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="74" t="s">
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="68"/>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="72" t="s">
         <v>518</v>
       </c>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-    </row>
-    <row r="39" customFormat="false" ht="409" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="397" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="76" t="s">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B41" s="74" t="s">
         <v>506</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-    </row>
-    <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="4" t="s">
         <v>519</v>
       </c>
@@ -4885,39 +4862,39 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="74" t="s">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="72" t="s">
         <v>520</v>
       </c>
-      <c r="C43" s="74"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-    </row>
-    <row r="44" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="75" t="s">
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="73" t="s">
         <v>521</v>
       </c>
-      <c r="C44" s="75"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
-    </row>
-    <row r="45" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="75" t="s">
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="73" t="s">
         <v>522</v>
       </c>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-    </row>
-    <row r="46" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="76" t="s">
+      <c r="C45" s="73"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="73"/>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="74" t="s">
         <v>523</v>
       </c>
-      <c r="C46" s="76"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="76"/>
-    </row>
-    <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C46" s="74"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="4" t="s">
         <v>524</v>
       </c>
@@ -4925,23 +4902,23 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="74" t="s">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="72" t="s">
         <v>525</v>
       </c>
-      <c r="C48" s="74"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-    </row>
-    <row r="49" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="76" t="s">
+      <c r="C48" s="72"/>
+      <c r="D48" s="72"/>
+      <c r="E48" s="72"/>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B49" s="74" t="s">
         <v>526</v>
       </c>
-      <c r="C49" s="76"/>
-      <c r="D49" s="76"/>
-      <c r="E49" s="76"/>
-    </row>
-    <row r="50" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C49" s="74"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="4" t="s">
         <v>527</v>
       </c>
@@ -4949,23 +4926,23 @@
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="74" t="s">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B51" s="72" t="s">
         <v>528</v>
       </c>
-      <c r="C51" s="74"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-    </row>
-    <row r="52" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="76" t="s">
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B52" s="74" t="s">
         <v>529</v>
       </c>
-      <c r="C52" s="76"/>
-      <c r="D52" s="76"/>
-      <c r="E52" s="76"/>
-    </row>
-    <row r="53" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C52" s="74"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
+    </row>
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="4" t="s">
         <v>530</v>
       </c>
@@ -4973,21 +4950,21 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="74" t="s">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B54" s="72" t="s">
         <v>531</v>
       </c>
-      <c r="C54" s="74"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-    </row>
-    <row r="55" customFormat="false" ht="409" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C54" s="72"/>
+      <c r="D54" s="72"/>
+      <c r="E54" s="72"/>
+    </row>
+    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="397" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -5041,7 +5018,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5053,10 +5029,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="A10:G13 B17"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.78125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
@@ -5320,10 +5296,10 @@
   <dimension ref="B1:F33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A10:G13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="42.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.22"/>
@@ -5342,138 +5318,138 @@
       <c r="F1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="68" t="s">
         <v>548</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" customFormat="false" ht="43" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="72" t="s">
         <v>549</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="75" t="s">
         <v>550</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="68" t="s">
         <v>551</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
     </row>
     <row r="6" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
     </row>
     <row r="7" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="77" t="s">
         <v>553</v>
       </c>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="8" t="s">
         <v>554</v>
       </c>
-      <c r="D7" s="80"/>
-      <c r="E7" s="81" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="78" t="s">
         <v>555</v>
       </c>
-      <c r="F7" s="81"/>
+      <c r="F7" s="78"/>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="68" t="s">
         <v>556</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
     </row>
     <row r="9" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="72" t="s">
         <v>557</v>
       </c>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
     </row>
     <row r="10" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
         <v>558</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="82" t="n">
+      <c r="D10" s="79" t="n">
         <v>1600</v>
       </c>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
     </row>
     <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>559</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
     </row>
     <row r="12" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="74" t="s">
         <v>560</v>
       </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
       <c r="F12" s="6" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="72" t="s">
         <v>562</v>
       </c>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
     </row>
     <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="68" t="s">
         <v>563</v>
       </c>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="72" t="s">
         <v>564</v>
       </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
     </row>
     <row r="16" customFormat="false" ht="409" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="3"/>
@@ -5499,13 +5475,13 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="72" t="s">
         <v>566</v>
       </c>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
@@ -5517,13 +5493,13 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="74" t="s">
+      <c r="B21" s="72" t="s">
         <v>568</v>
       </c>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
     </row>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="4" t="s">
@@ -5535,13 +5511,13 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="72" t="s">
         <v>570</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
     </row>
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="4" t="s">
@@ -5553,13 +5529,13 @@
       <c r="F24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="80" t="s">
         <v>572</v>
       </c>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
     </row>
     <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="4" t="s">
@@ -5571,13 +5547,13 @@
       <c r="F26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="72" t="s">
         <v>574</v>
       </c>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
     </row>
     <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="4" t="s">
@@ -5589,13 +5565,13 @@
       <c r="F28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="74" t="s">
+      <c r="B29" s="72" t="s">
         <v>576</v>
       </c>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
     </row>
     <row r="30" customFormat="false" ht="409" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="3"/>
@@ -5612,22 +5588,22 @@
       <c r="F31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="84" t="s">
+      <c r="B32" s="81" t="s">
         <v>577</v>
       </c>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="81"/>
     </row>
     <row r="33" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="84" t="s">
+      <c r="B33" s="81" t="s">
         <v>578</v>
       </c>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -5682,10 +5658,10 @@
   <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K49" activeCellId="1" sqref="A10:G13 K49"/>
+      <selection pane="topLeft" activeCell="K49" activeCellId="0" sqref="K49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.83"/>
@@ -7770,11 +7746,11 @@
   </sheetPr>
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="A10:G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.78125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
@@ -7818,7 +7794,7 @@
       </c>
       <c r="P1" s="33" t="str">
         <f aca="false">CONCATENATE(A1,B1,C1,D1,E1,F1,G1,H1,I1,J1,K1,L1,M1,N1,O1)</f>
-        <v>&lt;a href="#" data-popup="#popup_130" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Хіросіма&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 50 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_130" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Хіросіма&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 50 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q1" s="18" t="s">
         <v>155</v>
@@ -7870,7 +7846,7 @@
       </c>
       <c r="P2" s="33" t="str">
         <f aca="false">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2)</f>
-        <v>&lt;a href="#" data-popup="#popup_131" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лексус&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 50 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;110 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_131" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лексус&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 50 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;110 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q2" s="18" t="s">
         <v>155</v>
@@ -7922,7 +7898,7 @@
       </c>
       <c r="P3" s="33" t="str">
         <f aca="false">CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3)</f>
-        <v>&lt;a href="#" data-popup="#popup_132" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Б-52&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 50 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_132" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Б-52&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 50 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q3" s="18" t="s">
         <v>155</v>
@@ -8240,10 +8216,10 @@
   <dimension ref="A1:R265"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A138" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C154" activeCellId="1" sqref="A10:G13 C154"/>
+      <selection pane="topLeft" activeCell="C154" activeCellId="0" sqref="C154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="67.12"/>
@@ -8307,7 +8283,7 @@
       </c>
       <c r="N2" s="0" t="str">
         <f aca="false">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2)</f>
-        <v>&lt;a href="#" data-popup="#popup_74" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Рис з овочами&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_74" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Рис з овочами&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8352,7 +8328,7 @@
       </c>
       <c r="N3" s="0" t="str">
         <f aca="false">CONCATENATE(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3)</f>
-        <v>&lt;a href="#" data-popup="#popup_75" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Овочі гриль&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_75" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Овочі гриль&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8397,7 +8373,7 @@
       </c>
       <c r="N4" s="0" t="str">
         <f aca="false">CONCATENATE(A4,B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4,M4)</f>
-        <v>&lt;a href="#" data-popup="#popup_76" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лаваш з сиром&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_76" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лаваш з сиром&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8442,7 +8418,7 @@
       </c>
       <c r="N5" s="0" t="str">
         <f aca="false">CONCATENATE(A5,B5,C5,D5,E5,F5,G5,H5,I5,J5,K5,L5,M5)</f>
-        <v>&lt;a href="#" data-popup="#popup_77" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лаваш з курячим філе та томатами&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;135 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_77" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лаваш з курячим філе та томатами&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;135 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8487,7 +8463,7 @@
       </c>
       <c r="N6" s="0" t="str">
         <f aca="false">CONCATENATE(A6,B6,C6,D6,E6,F6,G6,H6,I6,J6,K6,L6,M6)</f>
-        <v>&lt;a href="#" data-popup="#popup_78" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лаваш з телятиною та соленим огірком&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;160 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_78" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лаваш з телятиною та соленим огірком&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;160 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8532,7 +8508,7 @@
       </c>
       <c r="N7" s="0" t="str">
         <f aca="false">CONCATENATE(A7,B7,C7,D7,E7,F7,G7,H7,I7,J7,K7,L7,M7)</f>
-        <v>&lt;a href="#" data-popup="#popup_79" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Картопля печена з салом та бринзою&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;80 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_79" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Картопля печена з салом та бринзою&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;80 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8577,7 +8553,7 @@
       </c>
       <c r="N8" s="0" t="str">
         <f aca="false">CONCATENATE(A8,B8,C8,D8,E8,F8,G8,H8,I8,J8,K8,L8,M8)</f>
-        <v>&lt;a href="#" data-popup="#popup_80" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Картопля по домашньому&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;60 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_80" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Картопля по домашньому&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;60 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8622,7 +8598,7 @@
       </c>
       <c r="N9" s="0" t="str">
         <f aca="false">CONCATENATE(A9,B9,C9,D9,E9,F9,G9,H9,I9,J9,K9,L9,M9)</f>
-        <v>&lt;a href="#" data-popup="#popup_81" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Палента з соусом Песто&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;70 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_81" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Палента з соусом Песто&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;70 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8667,7 +8643,7 @@
       </c>
       <c r="N10" s="0" t="str">
         <f aca="false">CONCATENATE(A10,B10,C10,D10,E10,F10,G10,H10,I10,J10,K10,L10,M10)</f>
-        <v>&lt;a href="#" data-popup="#popup_82" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Шпинатна подушка&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;90 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_82" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Шпинатна подушка&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;90 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8712,7 +8688,7 @@
       </c>
       <c r="N11" s="0" t="str">
         <f aca="false">CONCATENATE(A11,B11,C11,D11,E11,F11,G11,H11,I11,J11,K11,L11,M11)</f>
-        <v>&lt;a href="#" data-popup="#popup_83" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Спаржа&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 100 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;90 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_83" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Спаржа&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 100 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;90 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9232,7 +9208,7 @@
       </c>
       <c r="N24" s="0" t="str">
         <f aca="false">CONCATENATE(A24,B24,C24,D24,E24,F24,G24,H24,I24,J24,K24,L24,M24)</f>
-        <v>&lt;a href="#" data-popup="#popup_84" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Фондан шоколадний&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 140 г / 40 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;150 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_84" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Фондан шоколадний&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 140 г / 40 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;150 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9277,7 +9253,7 @@
       </c>
       <c r="N25" s="0" t="str">
         <f aca="false">CONCATENATE(A25,B25,C25,D25,E25,F25,G25,H25,I25,J25,K25,L25,M25)</f>
-        <v>&lt;a href="#" data-popup="#popup_85" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лимонний тарт&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 140 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;150 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_85" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лимонний тарт&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 140 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;150 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9322,7 +9298,7 @@
       </c>
       <c r="N26" s="0" t="str">
         <f aca="false">CONCATENATE(A26,B26,C26,D26,E26,F26,G26,H26,I26,J26,K26,L26,M26)</f>
-        <v>&lt;a href="#" data-popup="#popup_86" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Чізкейк&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 140 г / 40 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_86" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Чізкейк&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 140 г / 40 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9367,7 +9343,7 @@
       </c>
       <c r="N27" s="0" t="str">
         <f aca="false">CONCATENATE(A27,B27,C27,D27,E27,F27,G27,H27,I27,J27,K27,L27,M27)</f>
-        <v>&lt;a href="#" data-popup="#popup_87" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Штрудель&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;90 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_87" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Штрудель&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;90 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9412,7 +9388,7 @@
       </c>
       <c r="N28" s="0" t="str">
         <f aca="false">CONCATENATE(A28,B28,C28,D28,E28,F28,G28,H28,I28,J28,K28,L28,M28)</f>
-        <v>&lt;a href="#" data-popup="#popup_88" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Млинці з творогом&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_88" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Млинці з творогом&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9457,7 +9433,7 @@
       </c>
       <c r="N29" s="0" t="str">
         <f aca="false">CONCATENATE(A29,B29,C29,D29,E29,F29,G29,H29,I29,J29,K29,L29,M29)</f>
-        <v>&lt;a href="#" data-popup="#popup_89" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Млинці з медом та горіхами&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_89" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Млинці з медом та горіхами&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;95 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9502,7 +9478,7 @@
       </c>
       <c r="N30" s="0" t="str">
         <f aca="false">CONCATENATE(A30,B30,C30,D30,E30,F30,G30,H30,I30,J30,K30,L30,M30)</f>
-        <v>&lt;a href="#" data-popup="#popup_90" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Сирники з сметаною&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;130 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_90" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Сирники з сметаною&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;130 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9547,7 +9523,7 @@
       </c>
       <c r="N31" s="0" t="str">
         <f aca="false">CONCATENATE(A31,B31,C31,D31,E31,F31,G31,H31,I31,J31,K31,L31,M31)</f>
-        <v>&lt;a href="#" data-popup="#popup_91" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Мілкшейк вершковий&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_91" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Мілкшейк вершковий&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9592,7 +9568,7 @@
       </c>
       <c r="N32" s="0" t="str">
         <f aca="false">CONCATENATE(A32,B32,C32,D32,E32,F32,G32,H32,I32,J32,K32,L32,M32)</f>
-        <v>&lt;a href="#" data-popup="#popup_92" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Мілкшейк шоколадний&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_92" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Мілкшейк шоколадний&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 г&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9635,7 +9611,7 @@
       </c>
       <c r="N33" s="0" t="str">
         <f aca="false">CONCATENATE(A33,B33,C33,D33,E33,F33,G33,H33,I33,J33,K33,L33,M33)</f>
-        <v>&lt;a href="#" data-popup="#popup_93" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Мілкшейк ягідний&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага &lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_93" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Мілкшейк ягідний&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага &lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="36" s="45" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10131,7 +10107,7 @@
       </c>
       <c r="N49" s="0" t="str">
         <f aca="false">CONCATENATE(A49,B49,C49,D49,E49,F49,G49,H49,I49,J49,K49,L49,M49)</f>
-        <v>&lt;a href="#" data-popup="#popup_94" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Рістрето&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;25 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_94" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Рістрето&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;25 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10173,7 +10149,7 @@
       </c>
       <c r="N50" s="0" t="str">
         <f aca="false">CONCATENATE(A50,B50,C50,D50,E50,F50,G50,H50,I50,J50,K50,L50,M50)</f>
-        <v>&lt;a href="#" data-popup="#popup_95" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Рістрето без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;30 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_95" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Рістрето без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;30 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10215,7 +10191,7 @@
       </c>
       <c r="N51" s="0" t="str">
         <f aca="false">CONCATENATE(A51,B51,C51,D51,E51,F51,G51,H51,I51,J51,K51,L51,M51)</f>
-        <v>&lt;a href="#" data-popup="#popup_96" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Еспресо&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;25 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_96" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Еспресо&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;25 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10257,7 +10233,7 @@
       </c>
       <c r="N52" s="0" t="str">
         <f aca="false">CONCATENATE(A52,B52,C52,D52,E52,F52,G52,H52,I52,J52,K52,L52,M52)</f>
-        <v>&lt;a href="#" data-popup="#popup_97" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Еспресо без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;30 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_97" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Еспресо без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;30 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10299,7 +10275,7 @@
       </c>
       <c r="N53" s="0" t="str">
         <f aca="false">CONCATENATE(A53,B53,C53,D53,E53,F53,G53,H53,I53,J53,K53,L53,M53)</f>
-        <v>&lt;a href="#" data-popup="#popup_98" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Американо&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;25 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_98" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Американо&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;25 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10341,7 +10317,7 @@
       </c>
       <c r="N54" s="0" t="str">
         <f aca="false">CONCATENATE(A54,B54,C54,D54,E54,F54,G54,H54,I54,J54,K54,L54,M54)</f>
-        <v>&lt;a href="#" data-popup="#popup_99" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Американо без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;30 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_99" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Американо без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;30 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10383,7 +10359,7 @@
       </c>
       <c r="N55" s="0" t="str">
         <f aca="false">CONCATENATE(A55,B55,C55,D55,E55,F55,G55,H55,I55,J55,K55,L55,M55)</f>
-        <v>&lt;a href="#" data-popup="#popup_100" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Капучіно &lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;45 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_100" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Капучіно &lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;45 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10428,7 +10404,7 @@
       </c>
       <c r="N56" s="0" t="str">
         <f aca="false">CONCATENATE(A56,B56,C56,D56,E56,F56,G56,H56,I56,J56,K56,L56,M56)</f>
-        <v>&lt;a href="#" data-popup="#popup_101" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Капучіно на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;65 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_101" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Капучіно на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;65 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10470,7 +10446,7 @@
       </c>
       <c r="N57" s="0" t="str">
         <f aca="false">CONCATENATE(A57,B57,C57,D57,E57,F57,G57,H57,I57,J57,K57,L57,M57)</f>
-        <v>&lt;a href="#" data-popup="#popup_102" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Капучіно без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;50 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_102" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Капучіно без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;50 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10515,7 +10491,7 @@
       </c>
       <c r="N58" s="0" t="str">
         <f aca="false">CONCATENATE(A58,B58,C58,D58,E58,F58,G58,H58,I58,J58,K58,L58,M58)</f>
-        <v>&lt;a href="#" data-popup="#popup_103" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Капучіно без кофеїну на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;70 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_103" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Капучіно без кофеїну на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;70 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10560,7 +10536,7 @@
       </c>
       <c r="N59" s="0" t="str">
         <f aca="false">CONCATENATE(A59,B59,C59,D59,E59,F59,G59,H59,I59,J59,K59,L59,M59)</f>
-        <v>&lt;a href="#" data-popup="#popup_104" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лате&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;50 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_104" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лате&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;50 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10605,7 +10581,7 @@
       </c>
       <c r="N60" s="0" t="str">
         <f aca="false">CONCATENATE(A60,B60,C60,D60,E60,F60,G60,H60,I60,J60,K60,L60,M60)</f>
-        <v>&lt;a href="#" data-popup="#popup_105" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лате на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;70 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_105" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лате на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;70 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10650,7 +10626,7 @@
       </c>
       <c r="N61" s="0" t="str">
         <f aca="false">CONCATENATE(A61,B61,C61,D61,E61,F61,G61,H61,I61,J61,K61,L61,M61)</f>
-        <v>&lt;a href="#" data-popup="#popup_106" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лате без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;55 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_106" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лате без кофеїну&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;55 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10695,7 +10671,7 @@
       </c>
       <c r="N62" s="0" t="str">
         <f aca="false">CONCATENATE(A62,B62,C62,D62,E62,F62,G62,H62,I62,J62,K62,L62,M62)</f>
-        <v>&lt;a href="#" data-popup="#popup_107" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лате без кофеїну на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;75 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_107" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Лате без кофеїну на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;75 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10740,7 +10716,7 @@
       </c>
       <c r="N63" s="0" t="str">
         <f aca="false">CONCATENATE(A63,B63,C63,D63,E63,F63,G63,H63,I63,J63,K63,L63,M63)</f>
-        <v>&lt;a href="#" data-popup="#popup_108" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Фраппе&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;80 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_108" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Фраппе&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;80 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10785,7 +10761,7 @@
       </c>
       <c r="N64" s="0" t="str">
         <f aca="false">CONCATENATE(A64,B64,C64,D64,E64,F64,G64,H64,I64,J64,K64,L64,M64)</f>
-        <v>&lt;a href="#" data-popup="#popup_109" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Фрапе на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_109" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Фрапе на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10830,7 +10806,7 @@
       </c>
       <c r="N65" s="0" t="str">
         <f aca="false">CONCATENATE(A65,B65,C65,D65,E65,F65,G65,H65,I65,J65,K65,L65,M65)</f>
-        <v>&lt;a href="#" data-popup="#popup_110" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Фрапе без кофеїну на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;125 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_110" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Фрапе без кофеїну на соєвому молоці&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;125 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10875,7 +10851,7 @@
       </c>
       <c r="N66" s="0" t="str">
         <f aca="false">CONCATENATE(A66,B66,C66,D66,E66,F66,G66,H66,I66,J66,K66,L66,M66)</f>
-        <v>&lt;a href="#" data-popup="#popup_111" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Какао&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;60 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_111" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Какао&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;60 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="19.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14603,7 +14579,7 @@
       </c>
       <c r="P220" s="33" t="str">
         <f aca="false">CONCATENATE(A220,B220,C220,D220,E220,F220,G220,H220,I220,J220,K220,L220,M220,N220,O220)</f>
-        <v>&lt;a href="#" data-popup="#popup_112" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Long Island Ice Tee&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 350 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;190 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_112" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Long Island Ice Tee&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 350 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;190 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q220" s="18" t="s">
         <v>155</v>
@@ -14655,7 +14631,7 @@
       </c>
       <c r="P221" s="33" t="str">
         <f aca="false">CONCATENATE(A221,B221,C221,D221,E221,F221,G221,H221,I221,J221,K221,L221,M221,N221,O221)</f>
-        <v>&lt;a href="#" data-popup="#popup_113" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Berry Killer&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;180 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_113" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Berry Killer&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;180 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q221" s="18" t="s">
         <v>155</v>
@@ -14707,7 +14683,7 @@
       </c>
       <c r="P222" s="33" t="str">
         <f aca="false">CONCATENATE(A222,B222,C222,D222,E222,F222,G222,H222,I222,J222,K222,L222,M222,N222,O222)</f>
-        <v>&lt;a href="#" data-popup="#popup_114" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Blue Lagoon&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 350 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;150 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_114" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Blue Lagoon&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 350 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;150 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q222" s="18" t="s">
         <v>155</v>
@@ -14759,7 +14735,7 @@
       </c>
       <c r="P223" s="33" t="str">
         <f aca="false">CONCATENATE(A223,B223,C223,D223,E223,F223,G223,H223,I223,J223,K223,L223,M223,N223,O223)</f>
-        <v>&lt;a href="#" data-popup="#popup_115" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Cosmopolitan&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 100 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_115" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Cosmopolitan&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 100 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;120 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q223" s="18" t="s">
         <v>155</v>
@@ -14812,7 +14788,7 @@
       </c>
       <c r="P224" s="33" t="str">
         <f aca="false">CONCATENATE(A224,B224,C224,D224,E224,F224,G224,H224,I224,J224,K224,L224,M224,N224,O224)</f>
-        <v>&lt;a href="#" data-popup="#popup_116" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Sex on Beach&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 350 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;160 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_116" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Sex on Beach&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 350 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;160 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q224" s="18" t="s">
         <v>155</v>
@@ -14864,7 +14840,7 @@
       </c>
       <c r="P225" s="33" t="str">
         <f aca="false">CONCATENATE(A225,B225,C225,D225,E225,F225,G225,H225,I225,J225,K225,L225,M225,N225,O225)</f>
-        <v>&lt;a href="#" data-popup="#popup_117" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Hungarian Merry&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;90 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_117" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Hungarian Merry&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;90 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q225" s="18" t="s">
         <v>155</v>
@@ -14916,7 +14892,7 @@
       </c>
       <c r="P226" s="33" t="str">
         <f aca="false">CONCATENATE(A226,B226,C226,D226,E226,F226,G226,H226,I226,J226,K226,L226,M226,N226,O226)</f>
-        <v>&lt;a href="#" data-popup="#popup_118" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Pina Colada&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 350 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;180 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_118" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Pina Colada&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 350 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;180 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q226" s="18" t="s">
         <v>155</v>
@@ -14968,7 +14944,7 @@
       </c>
       <c r="P227" s="33" t="str">
         <f aca="false">CONCATENATE(A227,B227,C227,D227,E227,F227,G227,H227,I227,J227,K227,L227,M227,N227,O227)</f>
-        <v>&lt;a href="#" data-popup="#popup_119" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Mojito&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;160 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_119" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Mojito&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;160 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q227" s="18" t="s">
         <v>155</v>
@@ -15020,7 +14996,7 @@
       </c>
       <c r="P228" s="33" t="str">
         <f aca="false">CONCATENATE(A228,B228,C228,D228,E228,F228,G228,H228,I228,J228,K228,L228,M228,N228,O228)</f>
-        <v>&lt;a href="#" data-popup="#popup_120" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Jin-Tonic&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;145 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_120" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Jin-Tonic&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 200 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;145 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q228" s="18" t="s">
         <v>155</v>
@@ -15072,7 +15048,7 @@
       </c>
       <c r="P229" s="33" t="str">
         <f aca="false">CONCATENATE(A229,B229,C229,D229,E229,F229,G229,H229,I229,J229,K229,L229,M229,N229,O229)</f>
-        <v>&lt;a href="#" data-popup="#popup_121" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Margarita&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 175 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;170 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_121" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Margarita&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 175 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;170 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q229" s="18" t="s">
         <v>155</v>
@@ -15124,7 +15100,7 @@
       </c>
       <c r="P230" s="33" t="str">
         <f aca="false">CONCATENATE(A230,B230,C230,D230,E230,F230,G230,H230,I230,J230,K230,L230,M230,N230,O230)</f>
-        <v>&lt;a href="#" data-popup="#popup_122" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Tequila Sunrise&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 325 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;170 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_122" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Tequila Sunrise&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 325 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;170 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q230" s="18" t="s">
         <v>155</v>
@@ -15176,7 +15152,7 @@
       </c>
       <c r="P231" s="33" t="str">
         <f aca="false">CONCATENATE(A231,B231,C231,D231,E231,F231,G231,H231,I231,J231,K231,L231,M231,N231,O231)</f>
-        <v>&lt;a href="#" data-popup="#popup_123" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Strawberry Punch&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 230 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;180 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_123" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Strawberry Punch&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 230 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;180 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q231" s="18" t="s">
         <v>155</v>
@@ -15228,7 +15204,7 @@
       </c>
       <c r="P232" s="33" t="str">
         <f aca="false">CONCATENATE(A232,B232,C232,D232,E232,F232,G232,H232,I232,J232,K232,L232,M232,N232,O232)</f>
-        <v>&lt;a href="#" data-popup="#popup_124" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Aperol&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;140 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_124" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Aperol&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;140 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q232" s="18" t="s">
         <v>155</v>
@@ -15280,7 +15256,7 @@
       </c>
       <c r="P233" s="33" t="str">
         <f aca="false">CONCATENATE(A233,B233,C233,D233,E233,F233,G233,H233,I233,J233,K233,L233,M233,N233,O233)</f>
-        <v>&lt;a href="#" data-popup="#popup_125" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Martini Royal&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 175 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;135 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_125" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Martini Royal&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 175 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;135 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q233" s="18" t="s">
         <v>155</v>
@@ -15332,7 +15308,7 @@
       </c>
       <c r="P234" s="33" t="str">
         <f aca="false">CONCATENATE(A234,B234,C234,D234,E234,F234,G234,H234,I234,J234,K234,L234,M234,N234,O234)</f>
-        <v>&lt;a href="#" data-popup="#popup_126" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Penicillin&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 150 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;165 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_126" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Penicillin&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 150 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;165 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q234" s="18" t="s">
         <v>155</v>
@@ -15384,7 +15360,7 @@
       </c>
       <c r="P235" s="33" t="str">
         <f aca="false">CONCATENATE(A235,B235,C235,D235,E235,F235,G235,H235,I235,J235,K235,L235,M235,N235,O235)</f>
-        <v>&lt;a href="#" data-popup="#popup_127" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Hugo Sprits&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;140 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_127" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Hugo Sprits&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 250 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;140 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q235" s="18" t="s">
         <v>155</v>
@@ -15436,7 +15412,7 @@
       </c>
       <c r="P236" s="33" t="str">
         <f aca="false">CONCATENATE(A236,B236,C236,D236,E236,F236,G236,H236,I236,J236,K236,L236,M236,N236,O236)</f>
-        <v>&lt;a href="#" data-popup="#popup_128" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Negroni&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 100 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;140 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_128" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Negroni&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 100 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;140 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q236" s="18" t="s">
         <v>155</v>
@@ -15488,7 +15464,7 @@
       </c>
       <c r="P237" s="33" t="str">
         <f aca="false">CONCATENATE(A237,B237,C237,D237,E237,F237,G237,H237,I237,J237,K237,L237,M237,N237,O237)</f>
-        <v>&lt;a href="#" data-popup="#popup_129" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Berry whiskey&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 100 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;170 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt; </v>
+        <v>&lt;a href="#" data-popup="#popup_129" class="category-menu__item item-category-menu"&gt;&lt;div class="item-category-menu__content"&gt;&lt;div class="item-category-menu__info"&gt;&lt;h5 class="item-category-menu__label"&gt;Berry whiskey&lt;/h5&gt;&lt;div class="item-category-menu__description"&gt;&lt;/div&gt;&lt;div class="item-category-menu__weigth"&gt;Вага 100 мл&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__price"&gt;170 грн.&lt;/div&gt;&lt;/div&gt;&lt;div class="item-category-menu__image-ibg"&gt;&lt;picture&gt;&lt;source srcset="img/menu-page/01.webp" type="image/webp"&gt;&lt;img src="img/menu-page/01.jpg" alt="image product"&gt;&lt;/picture&gt;&lt;/div&gt;&lt;/a&gt;</v>
       </c>
       <c r="Q237" s="18" t="s">
         <v>155</v>
@@ -16453,10 +16429,10 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="1" sqref="A10:G13 F34"/>
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.89"/>
@@ -16566,31 +16542,31 @@
         <v>53</v>
       </c>
       <c r="F8" s="53"/>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="H8" s="54"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>418</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="54" t="s">
         <v>227</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
     </row>
     <row r="10" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="55" t="s">
         <v>419</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
       <c r="E10" s="53"/>
       <c r="F10" s="53"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="13" t="s">
@@ -16732,14 +16708,14 @@
         <v>420</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="58" t="s">
+      <c r="E20" s="56"/>
+      <c r="F20" s="57" t="s">
         <v>245</v>
       </c>
-      <c r="G20" s="58"/>
+      <c r="G20" s="57"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="18.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16747,10 +16723,10 @@
         <v>246</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="59" t="s">
+      <c r="D21" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="E21" s="59"/>
+      <c r="E21" s="58"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="3"/>
@@ -16760,10 +16736,10 @@
         <v>247</v>
       </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="58" t="s">
         <v>203</v>
       </c>
-      <c r="E22" s="59"/>
+      <c r="E22" s="58"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="3"/>
@@ -16773,10 +16749,10 @@
         <v>248</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="59" t="s">
+      <c r="D23" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="E23" s="59"/>
+      <c r="E23" s="58"/>
       <c r="F23" s="52" t="s">
         <v>198</v>
       </c>
@@ -16788,10 +16764,10 @@
         <v>250</v>
       </c>
       <c r="C24" s="13"/>
-      <c r="D24" s="59" t="s">
+      <c r="D24" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="E24" s="59"/>
+      <c r="E24" s="58"/>
       <c r="F24" s="52" t="s">
         <v>230</v>
       </c>
@@ -16803,10 +16779,10 @@
         <v>251</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="59" t="s">
+      <c r="D25" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="E25" s="59"/>
+      <c r="E25" s="58"/>
       <c r="F25" s="52" t="s">
         <v>230</v>
       </c>
@@ -16818,10 +16794,10 @@
         <v>252</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="59" t="s">
+      <c r="D26" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="E26" s="59"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="52" t="s">
         <v>230</v>
       </c>
@@ -16833,10 +16809,10 @@
         <v>253</v>
       </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="59" t="s">
+      <c r="D27" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="E27" s="59"/>
+      <c r="E27" s="58"/>
       <c r="F27" s="52" t="s">
         <v>230</v>
       </c>
@@ -16859,10 +16835,10 @@
         <v>254</v>
       </c>
       <c r="C29" s="13"/>
-      <c r="D29" s="60" t="s">
+      <c r="D29" s="59" t="s">
         <v>255</v>
       </c>
-      <c r="E29" s="60"/>
+      <c r="E29" s="59"/>
       <c r="F29" s="52" t="s">
         <v>256</v>
       </c>
@@ -16874,10 +16850,10 @@
         <v>257</v>
       </c>
       <c r="C30" s="13"/>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="E30" s="60"/>
+      <c r="E30" s="59"/>
       <c r="F30" s="52" t="s">
         <v>258</v>
       </c>
@@ -16889,10 +16865,10 @@
         <v>259</v>
       </c>
       <c r="C31" s="13"/>
-      <c r="D31" s="60" t="s">
+      <c r="D31" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="E31" s="60"/>
+      <c r="E31" s="59"/>
       <c r="F31" s="52" t="s">
         <v>260</v>
       </c>
@@ -16904,10 +16880,10 @@
         <v>422</v>
       </c>
       <c r="C32" s="13"/>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="59" t="s">
         <v>262</v>
       </c>
-      <c r="E32" s="60"/>
+      <c r="E32" s="59"/>
       <c r="F32" s="52" t="s">
         <v>226</v>
       </c>
@@ -17216,10 +17192,10 @@
   <dimension ref="B1:G35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="1" sqref="A10:G13 D23"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="53.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.88"/>
@@ -17481,11 +17457,11 @@
         <v>431</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="61" t="s">
+      <c r="E22" s="60" t="s">
         <v>432</v>
       </c>
-      <c r="F22" s="61"/>
-      <c r="G22" s="62" t="s">
+      <c r="F22" s="60"/>
+      <c r="G22" s="61" t="s">
         <v>433</v>
       </c>
     </row>
@@ -17526,14 +17502,14 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="63" t="s">
+      <c r="C26" s="57"/>
+      <c r="D26" s="62" t="s">
         <v>436</v>
       </c>
-      <c r="E26" s="63"/>
+      <c r="E26" s="62"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
@@ -17721,10 +17697,10 @@
   <dimension ref="B1:E43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E41" activeCellId="1" sqref="A10:G13 E41"/>
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.89"/>
@@ -17745,7 +17721,7 @@
         <v>326</v>
       </c>
       <c r="C2" s="13"/>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E2" s="52" t="s">
@@ -17757,7 +17733,7 @@
         <v>327</v>
       </c>
       <c r="C3" s="13"/>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E3" s="52" t="s">
@@ -17769,7 +17745,7 @@
         <v>440</v>
       </c>
       <c r="C4" s="13"/>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E4" s="52" t="s">
@@ -17781,7 +17757,7 @@
         <v>329</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E5" s="52" t="s">
@@ -17793,7 +17769,7 @@
         <v>330</v>
       </c>
       <c r="C6" s="13"/>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E6" s="52" t="s">
@@ -17805,7 +17781,7 @@
         <v>331</v>
       </c>
       <c r="C7" s="13"/>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E7" s="52" t="s">
@@ -17817,7 +17793,7 @@
         <v>332</v>
       </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E8" s="52" t="s">
@@ -17829,7 +17805,7 @@
         <v>333</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E9" s="52" t="s">
@@ -17841,7 +17817,7 @@
         <v>334</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E10" s="52" t="s">
@@ -17853,7 +17829,7 @@
         <v>336</v>
       </c>
       <c r="C11" s="13"/>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E11" s="52" t="s">
@@ -17873,7 +17849,7 @@
         <v>305</v>
       </c>
       <c r="C13" s="13"/>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E13" s="52" t="s">
@@ -17885,7 +17861,7 @@
         <v>307</v>
       </c>
       <c r="C14" s="13"/>
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E14" s="52" t="s">
@@ -17897,7 +17873,7 @@
         <v>309</v>
       </c>
       <c r="C15" s="13"/>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E15" s="52" t="s">
@@ -17909,7 +17885,7 @@
         <v>310</v>
       </c>
       <c r="C16" s="13"/>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E16" s="52" t="s">
@@ -17921,7 +17897,7 @@
         <v>311</v>
       </c>
       <c r="C17" s="13"/>
-      <c r="D17" s="64" t="s">
+      <c r="D17" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E17" s="52" t="s">
@@ -17933,7 +17909,7 @@
         <v>312</v>
       </c>
       <c r="C18" s="13"/>
-      <c r="D18" s="64" t="s">
+      <c r="D18" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E18" s="52" t="s">
@@ -17953,7 +17929,7 @@
         <v>337</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="65" t="s">
+      <c r="D20" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E20" s="52" t="s">
@@ -17965,7 +17941,7 @@
         <v>340</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="65" t="s">
+      <c r="D21" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E21" s="52" t="s">
@@ -17977,7 +17953,7 @@
         <v>342</v>
       </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="65" t="s">
+      <c r="D22" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E22" s="52" t="s">
@@ -17989,7 +17965,7 @@
         <v>448</v>
       </c>
       <c r="C23" s="13"/>
-      <c r="D23" s="65" t="s">
+      <c r="D23" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E23" s="52" t="s">
@@ -18001,7 +17977,7 @@
         <v>345</v>
       </c>
       <c r="C24" s="13"/>
-      <c r="D24" s="65" t="s">
+      <c r="D24" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E24" s="52" t="s">
@@ -18013,7 +17989,7 @@
         <v>347</v>
       </c>
       <c r="C25" s="13"/>
-      <c r="D25" s="65" t="s">
+      <c r="D25" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E25" s="52" t="s">
@@ -18025,7 +18001,7 @@
         <v>349</v>
       </c>
       <c r="C26" s="13"/>
-      <c r="D26" s="65" t="s">
+      <c r="D26" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E26" s="52" t="s">
@@ -18037,7 +18013,7 @@
         <v>350</v>
       </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="65" t="s">
+      <c r="D27" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E27" s="52" t="s">
@@ -18049,7 +18025,7 @@
         <v>352</v>
       </c>
       <c r="C28" s="13"/>
-      <c r="D28" s="65" t="s">
+      <c r="D28" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E28" s="52" t="s">
@@ -18061,7 +18037,7 @@
         <v>354</v>
       </c>
       <c r="C29" s="13"/>
-      <c r="D29" s="65" t="s">
+      <c r="D29" s="64" t="s">
         <v>338</v>
       </c>
       <c r="E29" s="52" t="s">
@@ -18073,7 +18049,7 @@
         <v>355</v>
       </c>
       <c r="C30" s="13"/>
-      <c r="D30" s="65" t="s">
+      <c r="D30" s="64" t="s">
         <v>393</v>
       </c>
       <c r="E30" s="52" t="s">
@@ -18093,7 +18069,7 @@
         <v>356</v>
       </c>
       <c r="C32" s="13"/>
-      <c r="D32" s="64" t="s">
+      <c r="D32" s="63" t="s">
         <v>150</v>
       </c>
       <c r="E32" s="52" t="s">
@@ -18112,10 +18088,10 @@
       <c r="B34" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="63" t="s">
         <v>358</v>
       </c>
-      <c r="D34" s="64"/>
+      <c r="D34" s="63"/>
       <c r="E34" s="52" t="s">
         <v>359</v>
       </c>
@@ -18124,10 +18100,10 @@
       <c r="B35" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="53" t="s">
         <v>361</v>
       </c>
-      <c r="D35" s="66"/>
+      <c r="D35" s="53"/>
       <c r="E35" s="52" t="s">
         <v>228</v>
       </c>
@@ -18136,10 +18112,10 @@
       <c r="B36" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="63" t="s">
         <v>358</v>
       </c>
-      <c r="D36" s="64"/>
+      <c r="D36" s="63"/>
       <c r="E36" s="52" t="s">
         <v>363</v>
       </c>
@@ -18148,10 +18124,10 @@
       <c r="B37" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="C37" s="66" t="s">
+      <c r="C37" s="53" t="s">
         <v>365</v>
       </c>
-      <c r="D37" s="66"/>
+      <c r="D37" s="53"/>
       <c r="E37" s="52" t="s">
         <v>176</v>
       </c>
@@ -18160,10 +18136,10 @@
       <c r="B38" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="C38" s="66" t="s">
+      <c r="C38" s="53" t="s">
         <v>365</v>
       </c>
-      <c r="D38" s="66"/>
+      <c r="D38" s="53"/>
       <c r="E38" s="52" t="s">
         <v>157</v>
       </c>
@@ -18172,10 +18148,10 @@
       <c r="B39" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="C39" s="64" t="s">
+      <c r="C39" s="63" t="s">
         <v>358</v>
       </c>
-      <c r="D39" s="64"/>
+      <c r="D39" s="63"/>
       <c r="E39" s="52" t="s">
         <v>368</v>
       </c>
@@ -18184,10 +18160,10 @@
       <c r="B40" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="53" t="s">
         <v>370</v>
       </c>
-      <c r="D40" s="66"/>
+      <c r="D40" s="53"/>
       <c r="E40" s="52" t="s">
         <v>194</v>
       </c>
@@ -18196,10 +18172,10 @@
       <c r="B41" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="53" t="s">
         <v>361</v>
       </c>
-      <c r="D41" s="66"/>
+      <c r="D41" s="53"/>
       <c r="E41" s="52" t="s">
         <v>371</v>
       </c>
@@ -18279,10 +18255,10 @@
   <dimension ref="B1:E24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A10:G13 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="67.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.88"/>
@@ -18311,7 +18287,7 @@
       <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="65" t="s">
         <v>457</v>
       </c>
       <c r="C3" s="5"/>
@@ -18319,19 +18295,19 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="66" t="s">
         <v>458</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="62" t="s">
         <v>41</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>459</v>
       </c>
       <c r="C5" s="5"/>
@@ -18339,199 +18315,199 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="66" t="s">
         <v>460</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="67" t="s">
         <v>373</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="62" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="66" t="s">
         <v>461</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="67" t="s">
         <v>377</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="62" t="s">
         <v>61</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="66" t="s">
         <v>462</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="67" t="s">
         <v>373</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="62" t="s">
         <v>437</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="66" t="s">
         <v>463</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="67" t="s">
         <v>380</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="62" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="66" t="s">
         <v>464</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="67" t="s">
         <v>373</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="62" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>465</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="62" t="s">
         <v>437</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="66" t="s">
         <v>466</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="67" t="s">
         <v>380</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="62" t="s">
         <v>435</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="66" t="s">
         <v>467</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="67" t="s">
         <v>385</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="62" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="66" t="s">
         <v>468</v>
       </c>
-      <c r="C14" s="69" t="s">
+      <c r="C14" s="67" t="s">
         <v>387</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="62" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="66" t="s">
         <v>469</v>
       </c>
-      <c r="C15" s="69" t="s">
+      <c r="C15" s="67" t="s">
         <v>389</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="62" t="s">
         <v>41</v>
       </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="66" t="s">
         <v>470</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="D16" s="62" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="66" t="s">
         <v>471</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="67" t="s">
         <v>385</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="62" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="66" t="s">
         <v>472</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="67" t="s">
         <v>393</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="62" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="66" t="s">
         <v>473</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D19" s="62" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="66" t="s">
         <v>474</v>
       </c>
-      <c r="C20" s="69" t="s">
+      <c r="C20" s="67" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="63" t="s">
+      <c r="D20" s="62" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="68" t="s">
+      <c r="B21" s="66" t="s">
         <v>475</v>
       </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="67" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="63" t="s">
+      <c r="D21" s="62" t="s">
         <v>49</v>
       </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="65" t="s">
         <v>476</v>
       </c>
       <c r="C22" s="5"/>
@@ -18573,10 +18549,10 @@
   <dimension ref="B1:E24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A10:G13 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="58.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8"/>
@@ -18596,40 +18572,40 @@
       <c r="B2" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="68" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="69" t="s">
         <v>478</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="68" t="s">
         <v>426</v>
       </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="69" t="s">
         <v>479</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="68" t="s">
         <v>61</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="70" t="s">
         <v>480</v>
       </c>
       <c r="C5" s="5"/>
@@ -18648,10 +18624,10 @@
       <c r="B7" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="68" t="s">
         <v>434</v>
       </c>
       <c r="E7" s="3"/>
@@ -18660,10 +18636,10 @@
       <c r="B8" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="68" t="s">
         <v>434</v>
       </c>
       <c r="E8" s="3"/>
@@ -18672,10 +18648,10 @@
       <c r="B9" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="68" t="s">
         <v>49</v>
       </c>
       <c r="E9" s="3"/>
@@ -18684,10 +18660,10 @@
       <c r="B10" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="68" t="s">
         <v>434</v>
       </c>
       <c r="E10" s="3"/>
@@ -18704,7 +18680,7 @@
       <c r="B12" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="64" t="s">
         <v>483</v>
       </c>
       <c r="D12" s="52" t="s">
@@ -18716,7 +18692,7 @@
       <c r="B13" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="64" t="s">
         <v>373</v>
       </c>
       <c r="D13" s="52" t="s">
@@ -18728,7 +18704,7 @@
       <c r="B14" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="C14" s="65" t="s">
+      <c r="C14" s="64" t="s">
         <v>486</v>
       </c>
       <c r="D14" s="52" t="s">
@@ -18740,7 +18716,7 @@
       <c r="B15" s="13" t="s">
         <v>487</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="C15" s="64" t="s">
         <v>486</v>
       </c>
       <c r="D15" s="52" t="s">
@@ -18752,7 +18728,7 @@
       <c r="B16" s="13" t="s">
         <v>488</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="C16" s="64" t="s">
         <v>486</v>
       </c>
       <c r="D16" s="52" t="s">
@@ -18764,7 +18740,7 @@
       <c r="B17" s="13" t="s">
         <v>489</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="C17" s="64" t="s">
         <v>486</v>
       </c>
       <c r="D17" s="52" t="s">
@@ -18776,7 +18752,7 @@
       <c r="B18" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="64" t="s">
         <v>486</v>
       </c>
       <c r="D18" s="52" t="s">
@@ -18788,7 +18764,7 @@
       <c r="B19" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="C19" s="64" t="s">
         <v>486</v>
       </c>
       <c r="D19" s="52" t="s">
@@ -18800,7 +18776,7 @@
       <c r="B20" s="13" t="s">
         <v>492</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="64" t="s">
         <v>486</v>
       </c>
       <c r="D20" s="52" t="s">
@@ -18812,7 +18788,7 @@
       <c r="B21" s="13" t="s">
         <v>493</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="C21" s="64" t="s">
         <v>486</v>
       </c>
       <c r="D21" s="52" t="s">
@@ -18824,7 +18800,7 @@
       <c r="B22" s="13" t="s">
         <v>494</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="64" t="s">
         <v>486</v>
       </c>
       <c r="D22" s="52" t="s">

</xml_diff>